<commit_message>
zzf 费控 后台 2021-04-19 18:08:01
</commit_message>
<xml_diff>
--- a/PD/v5/assets/public/订单导入模板.xlsx
+++ b/PD/v5/assets/public/订单导入模板.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13433\Desktop\物流费控\物流费控\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13433\Desktop\工作\物流费控\导入模板\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4756F124-A002-4DEB-B183-39AEBB183CA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C9387-39B2-469E-9E4D-0933D8D5B605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1020" windowWidth="23040" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,104 +28,106 @@
     <t>订单码</t>
   </si>
   <si>
+    <t>合单费</t>
+  </si>
+  <si>
+    <t>中通基本运费</t>
+  </si>
+  <si>
+    <t>打包费</t>
+  </si>
+  <si>
+    <t>中通应收运费</t>
+  </si>
+  <si>
+    <t>京东反馈运费</t>
+  </si>
+  <si>
+    <t>京东计费重量</t>
+  </si>
+  <si>
+    <t>京东首重金额</t>
+  </si>
+  <si>
+    <t>京东应收运费</t>
+  </si>
+  <si>
+    <t>顺丰反馈的运费</t>
+  </si>
+  <si>
+    <t>顺丰计费重量</t>
+  </si>
+  <si>
+    <t>顺丰件类型</t>
+  </si>
+  <si>
+    <t>顺丰首重金额</t>
+  </si>
+  <si>
+    <t>顺丰应收运费</t>
+  </si>
+  <si>
+    <t>合计</t>
+  </si>
+  <si>
+    <t>优惠后合计</t>
+  </si>
+  <si>
+    <t>合并批次号</t>
+  </si>
+  <si>
+    <t>入库件数</t>
+  </si>
+  <si>
+    <t>质检机构</t>
+  </si>
+  <si>
+    <t>质检结果</t>
+  </si>
+  <si>
+    <t>复检结果</t>
+  </si>
+  <si>
+    <t>计划发货快递</t>
+  </si>
+  <si>
+    <t>实际发货快递</t>
+  </si>
+  <si>
+    <t>快递单号</t>
+  </si>
+  <si>
+    <t>收货省份</t>
+  </si>
+  <si>
+    <t>下单时间</t>
+  </si>
+  <si>
+    <t>入库时间</t>
+  </si>
+  <si>
+    <t>送检时间</t>
+  </si>
+  <si>
+    <t>质检完成时间</t>
+  </si>
+  <si>
+    <t>出库时间</t>
+  </si>
+  <si>
+    <t>*订单编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*商家ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>商家名称</t>
-  </si>
-  <si>
-    <t>订单履约状态</t>
-  </si>
-  <si>
-    <t>合单费</t>
-  </si>
-  <si>
-    <t>中通基本运费</t>
-  </si>
-  <si>
-    <t>打包费</t>
-  </si>
-  <si>
-    <t>中通应收运费</t>
-  </si>
-  <si>
-    <t>京东反馈运费</t>
-  </si>
-  <si>
-    <t>京东计费重量</t>
-  </si>
-  <si>
-    <t>京东首重金额</t>
-  </si>
-  <si>
-    <t>京东应收运费</t>
-  </si>
-  <si>
-    <t>顺丰反馈的运费</t>
-  </si>
-  <si>
-    <t>顺丰计费重量</t>
-  </si>
-  <si>
-    <t>顺丰件类型</t>
-  </si>
-  <si>
-    <t>顺丰首重金额</t>
-  </si>
-  <si>
-    <t>顺丰应收运费</t>
-  </si>
-  <si>
-    <t>合计</t>
-  </si>
-  <si>
-    <t>优惠后合计</t>
-  </si>
-  <si>
-    <t>合并批次号</t>
-  </si>
-  <si>
-    <t>入库件数</t>
-  </si>
-  <si>
-    <t>质检机构</t>
-  </si>
-  <si>
-    <t>质检结果</t>
-  </si>
-  <si>
-    <t>复检结果</t>
-  </si>
-  <si>
-    <t>计划发货快递</t>
-  </si>
-  <si>
-    <t>实际发货快递</t>
-  </si>
-  <si>
-    <t>快递单号</t>
-  </si>
-  <si>
-    <t>收货省份</t>
-  </si>
-  <si>
-    <t>下单时间</t>
-  </si>
-  <si>
-    <t>入库时间</t>
-  </si>
-  <si>
-    <t>送检时间</t>
-  </si>
-  <si>
-    <t>质检完成时间</t>
-  </si>
-  <si>
-    <t>出库时间</t>
-  </si>
-  <si>
-    <t>商家ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>订单编号</t>
+    <t>*订单履约状态</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -136,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +149,15 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -181,7 +192,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -198,6 +209,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -499,12 +513,12 @@
   <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="13.21875" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
@@ -538,106 +552,106 @@
   <sheetData>
     <row r="1" spans="1:34" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
zzf 费控 后台 2021-04-20 13:29:03
</commit_message>
<xml_diff>
--- a/PD/v5/assets/public/订单导入模板.xlsx
+++ b/PD/v5/assets/public/订单导入模板.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13433\Desktop\工作\物流费控\导入模板\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C9387-39B2-469E-9E4D-0933D8D5B605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF21637-931D-40BB-9DA0-89CACF1333A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1020" windowWidth="23040" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="订单导入模板" sheetId="1" r:id="rId1"/>
+    <sheet name="订单信息数据" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">订单导入模板!$A$1:$AH$6</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -28,6 +26,15 @@
     <t>订单码</t>
   </si>
   <si>
+    <t>*商家ID</t>
+  </si>
+  <si>
+    <t>商家名称</t>
+  </si>
+  <si>
+    <t>*订单履约状态</t>
+  </si>
+  <si>
     <t>合单费</t>
   </si>
   <si>
@@ -115,40 +122,171 @@
     <t>出库时间</t>
   </si>
   <si>
-    <t>*订单编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*商家ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商家名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*订单履约状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>订单编号</t>
+    </r>
+    <phoneticPr fontId="34" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+  <fonts count="37">
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -156,18 +294,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,54 +327,117 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -253,7 +451,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -269,7 +467,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -281,7 +479,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -295,12 +493,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -328,14 +526,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -363,6 +578,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,203 +737,148 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
-    <col min="11" max="11" width="19.21875" customWidth="1"/>
-    <col min="12" max="12" width="21.21875" customWidth="1"/>
-    <col min="13" max="13" width="19.5546875" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" customWidth="1"/>
-    <col min="15" max="16" width="18.88671875" customWidth="1"/>
-    <col min="17" max="17" width="17.77734375" customWidth="1"/>
-    <col min="18" max="18" width="19.5546875" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" customWidth="1"/>
-    <col min="20" max="20" width="16.44140625" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" customWidth="1"/>
-    <col min="23" max="23" width="15.21875" customWidth="1"/>
-    <col min="24" max="24" width="16.33203125" customWidth="1"/>
-    <col min="25" max="25" width="15.44140625" customWidth="1"/>
-    <col min="26" max="26" width="18.109375" customWidth="1"/>
-    <col min="27" max="27" width="18.21875" customWidth="1"/>
-    <col min="28" max="28" width="18.88671875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="13.88671875" customWidth="1"/>
-    <col min="30" max="33" width="17.109375" customWidth="1"/>
-    <col min="34" max="34" width="17.21875" customWidth="1"/>
+    <col min="1" max="34" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:34" ht="25.05" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="AG1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="AH1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="AB2" s="2"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="AB3" s="2"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="3"/>
-      <c r="AH3" s="3"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="AB4" s="2"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="AB5" s="2"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="AB6" s="2"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="AB2:AB1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-  </conditionalFormatting>
+  <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetData/>
+  <phoneticPr fontId="34" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>